<commit_message>
makes changes to metadata files following meeting with Nick and Melissa - mostly removing columns
</commit_message>
<xml_diff>
--- a/data-raw/metadata/delta_entry_catch_metadata.xlsx
+++ b/data-raw/metadata/delta_entry_catch_metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-delta-entry-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8DD5D7E-1566-894A-8BE3-FCE1AD073584}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{976F164B-10F2-1B42-BAE5-765CB1CA06D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="62">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -181,9 +181,6 @@
     <t>number of fish</t>
   </si>
   <si>
-    <t>atCaptureRun</t>
-  </si>
-  <si>
     <t>finalRun</t>
   </si>
   <si>
@@ -207,9 +204,6 @@
 "Largemouth bass", "Tule perch", "Unknown catfish/bullhead", 
 "Striped bass", "Red shiner", "Unknown bass (Micropterus)", "Unknown sculpin (Cottus)", 
 "American shad", "Prickly sculpin")</t>
-  </si>
-  <si>
-    <t>Run designation as determined in the field or as assigned at a later date. Levels = c("Not recorded", "Fall", "Spring", "Winter", NA).</t>
   </si>
   <si>
     <t>Origin/production type of the fish. Levels = c("Natural", "Hatchery").</t>
@@ -530,11 +524,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -613,7 +607,7 @@
         <v>44</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>18</v>
@@ -727,7 +721,7 @@
         <v>45</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>13</v>
@@ -800,10 +794,10 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>13</v>
@@ -838,10 +832,10 @@
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>13</v>
@@ -876,28 +870,38 @@
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>59</v>
+        <v>27</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
+      <c r="F9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="I9" s="2"/>
       <c r="J9" s="3"/>
       <c r="K9" s="2"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
+      <c r="L9" s="3">
+        <v>31</v>
+      </c>
+      <c r="M9" s="3">
+        <v>275</v>
+      </c>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
@@ -914,10 +918,10 @@
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>28</v>
@@ -941,10 +945,10 @@
       <c r="J10" s="3"/>
       <c r="K10" s="2"/>
       <c r="L10" s="3">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="M10" s="3">
-        <v>275</v>
+        <v>850</v>
       </c>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
@@ -962,10 +966,10 @@
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>28</v>
@@ -980,19 +984,19 @@
         <v>28</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="3"/>
       <c r="K11" s="2"/>
       <c r="L11" s="3">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="M11" s="3">
-        <v>850</v>
+        <v>116</v>
       </c>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
@@ -1010,37 +1014,33 @@
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
-      <c r="F12" s="3" t="s">
-        <v>28</v>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="5" t="s">
+        <v>40</v>
       </c>
-      <c r="G12" s="3" t="s">
-        <v>50</v>
+      <c r="K12" s="6"/>
+      <c r="L12" s="10">
+        <v>44582.531331018516</v>
       </c>
-      <c r="H12" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="I12" s="2"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="3">
-        <v>0</v>
-      </c>
-      <c r="M12" s="3">
-        <v>116</v>
+      <c r="M12" s="10">
+        <v>44720.427384259259</v>
       </c>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
@@ -1058,34 +1058,28 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
       <c r="I13" s="6"/>
-      <c r="J13" s="5" t="s">
-        <v>40</v>
-      </c>
+      <c r="J13" s="5"/>
       <c r="K13" s="6"/>
-      <c r="L13" s="10">
-        <v>44582.531331018516</v>
-      </c>
-      <c r="M13" s="10">
-        <v>44720.427384259259</v>
-      </c>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
@@ -1102,10 +1096,10 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>13</v>
@@ -1116,14 +1110,14 @@
       <c r="E14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
@@ -1140,10 +1134,10 @@
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>13</v>
@@ -1178,10 +1172,10 @@
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>13</v>
@@ -1219,7 +1213,7 @@
         <v>52</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>13</v>
@@ -1253,21 +1247,11 @@
       <c r="Z17" s="1"/>
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="A18" s="4"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="1"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
@@ -1290,20 +1274,20 @@
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
     </row>
-    <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="2"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
@@ -1318,7 +1302,7 @@
       <c r="Y19" s="1"/>
       <c r="Z19" s="1"/>
     </row>
-    <row r="20" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1330,8 +1314,8 @@
       <c r="I20" s="6"/>
       <c r="J20" s="5"/>
       <c r="K20" s="6"/>
-      <c r="L20" s="10"/>
-      <c r="M20" s="10"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
@@ -1352,14 +1336,14 @@
       <c r="C21" s="1"/>
       <c r="D21" s="2"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
@@ -1431,19 +1415,6 @@
       <c r="Z23" s="1"/>
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="4"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
@@ -1459,6 +1430,14 @@
       <c r="Z24" s="1"/>
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
@@ -1474,27 +1453,19 @@
       <c r="Z25" s="1"/>
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="2"/>
-      <c r="L26" s="3"/>
-      <c r="M26" s="3"/>
-      <c r="N26" s="1"/>
-      <c r="O26" s="1"/>
-      <c r="P26" s="1"/>
-      <c r="Q26" s="1"/>
-      <c r="R26" s="1"/>
-      <c r="S26" s="1"/>
-      <c r="T26" s="1"/>
-      <c r="U26" s="1"/>
-      <c r="V26" s="1"/>
-      <c r="W26" s="1"/>
-      <c r="X26" s="1"/>
-      <c r="Y26" s="1"/>
-      <c r="Z26" s="1"/>
+      <c r="N26" s="4"/>
+      <c r="O26" s="4"/>
+      <c r="P26" s="4"/>
+      <c r="Q26" s="4"/>
+      <c r="R26" s="4"/>
+      <c r="S26" s="4"/>
+      <c r="T26" s="4"/>
+      <c r="U26" s="4"/>
+      <c r="V26" s="4"/>
+      <c r="W26" s="4"/>
+      <c r="X26" s="4"/>
+      <c r="Y26" s="4"/>
+      <c r="Z26" s="4"/>
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="N27" s="4"/>
@@ -1512,19 +1483,19 @@
       <c r="Z27" s="4"/>
     </row>
     <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="N28" s="4"/>
-      <c r="O28" s="4"/>
-      <c r="P28" s="4"/>
-      <c r="Q28" s="4"/>
-      <c r="R28" s="4"/>
-      <c r="S28" s="4"/>
-      <c r="T28" s="4"/>
-      <c r="U28" s="4"/>
-      <c r="V28" s="4"/>
-      <c r="W28" s="4"/>
-      <c r="X28" s="4"/>
-      <c r="Y28" s="4"/>
-      <c r="Z28" s="4"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+      <c r="R28" s="1"/>
+      <c r="S28" s="1"/>
+      <c r="T28" s="1"/>
+      <c r="U28" s="1"/>
+      <c r="V28" s="1"/>
+      <c r="W28" s="1"/>
+      <c r="X28" s="1"/>
+      <c r="Y28" s="1"/>
+      <c r="Z28" s="1"/>
     </row>
     <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="N29" s="1"/>
@@ -1542,6 +1513,19 @@
       <c r="Z29" s="1"/>
     </row>
     <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="4"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
@@ -1641,7 +1625,7 @@
       <c r="Z33" s="1"/>
     </row>
     <row r="34" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="4"/>
+      <c r="A34" s="11"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="2"/>
@@ -1669,7 +1653,7 @@
       <c r="Z34" s="1"/>
     </row>
     <row r="35" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="11"/>
+      <c r="A35" s="12"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="2"/>
@@ -1697,7 +1681,7 @@
       <c r="Z35" s="1"/>
     </row>
     <row r="36" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="12"/>
+      <c r="A36" s="11"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="2"/>
@@ -1725,7 +1709,7 @@
       <c r="Z36" s="1"/>
     </row>
     <row r="37" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="11"/>
+      <c r="A37" s="12"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="2"/>
@@ -1753,7 +1737,7 @@
       <c r="Z37" s="1"/>
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="12"/>
+      <c r="A38" s="4"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="2"/>
@@ -2705,7 +2689,7 @@
       <c r="Z71" s="1"/>
     </row>
     <row r="72" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="4"/>
+      <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
       <c r="D72" s="2"/>
@@ -28632,50 +28616,22 @@
       <c r="Y997" s="1"/>
       <c r="Z997" s="1"/>
     </row>
-    <row r="998" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A998" s="1"/>
-      <c r="B998" s="1"/>
-      <c r="C998" s="1"/>
-      <c r="D998" s="2"/>
-      <c r="E998" s="1"/>
-      <c r="F998" s="3"/>
-      <c r="G998" s="3"/>
-      <c r="H998" s="3"/>
-      <c r="I998" s="2"/>
-      <c r="J998" s="3"/>
-      <c r="K998" s="2"/>
-      <c r="L998" s="3"/>
-      <c r="M998" s="3"/>
-      <c r="N998" s="1"/>
-      <c r="O998" s="1"/>
-      <c r="P998" s="1"/>
-      <c r="Q998" s="1"/>
-      <c r="R998" s="1"/>
-      <c r="S998" s="1"/>
-      <c r="T998" s="1"/>
-      <c r="U998" s="1"/>
-      <c r="V998" s="1"/>
-      <c r="W998" s="1"/>
-      <c r="X998" s="1"/>
-      <c r="Y998" s="1"/>
-      <c r="Z998" s="1"/>
-    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A36:A37"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C55:C998 C31:C43 C1:C24" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C54:C997 C30:C42 C1:C23" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E31:E998 E1:E24" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E30:E997 E1:E23" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F26 F31:F998 F1:F24" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F25 F30:F997 F1:F23" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"ratio,interval"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H26 H31:H998 H1:H24" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H25 H30:H997 H1:H23" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"natural,whole,integer,real"</formula1>
     </dataValidation>
   </dataValidations>
@@ -28739,7 +28695,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>44</v>

</xml_diff>

<commit_message>
aligning metadata with tables to validate xml
</commit_message>
<xml_diff>
--- a/data-raw/metadata/delta_entry_catch_metadata.xlsx
+++ b/data-raw/metadata/delta_entry_catch_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-delta-entry-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{976F164B-10F2-1B42-BAE5-765CB1CA06D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{397C9274-CAED-FA4F-90F4-8D4806710293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32580" yWindow="1620" windowWidth="17740" windowHeight="17140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="64">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -222,6 +222,12 @@
   </si>
   <si>
     <t>Run designation revised after field visit. Levels = c(NA, "Fall", "Spring", "Winter")</t>
+  </si>
+  <si>
+    <t>atCaptureRun</t>
+  </si>
+  <si>
+    <t>Run designation as determined in the field or as assigned at a later date. Levels = c("Not recorded", "Fall", "Spring", "Winter", "Late fall", "Not applicable (n/a)").</t>
   </si>
 </sst>
 </file>
@@ -524,11 +530,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z997"/>
+  <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7:XFD7"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -794,10 +800,10 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>24</v>
+        <v>62</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>13</v>
@@ -832,10 +838,10 @@
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>13</v>
@@ -870,38 +876,28 @@
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>30</v>
-      </c>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
       <c r="I9" s="2"/>
       <c r="J9" s="3"/>
       <c r="K9" s="2"/>
-      <c r="L9" s="3">
-        <v>31</v>
-      </c>
-      <c r="M9" s="3">
-        <v>275</v>
-      </c>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
@@ -918,10 +914,10 @@
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>28</v>
@@ -945,10 +941,10 @@
       <c r="J10" s="3"/>
       <c r="K10" s="2"/>
       <c r="L10" s="3">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="M10" s="3">
-        <v>850</v>
+        <v>275</v>
       </c>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
@@ -966,10 +962,10 @@
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>28</v>
@@ -984,19 +980,19 @@
         <v>28</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="3"/>
       <c r="K11" s="2"/>
       <c r="L11" s="3">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="M11" s="3">
-        <v>116</v>
+        <v>850</v>
       </c>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
@@ -1014,33 +1010,37 @@
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="5" t="s">
-        <v>40</v>
+      <c r="F12" s="3" t="s">
+        <v>28</v>
       </c>
-      <c r="K12" s="6"/>
-      <c r="L12" s="10">
-        <v>44582.531331018516</v>
+      <c r="G12" s="3" t="s">
+        <v>50</v>
       </c>
-      <c r="M12" s="10">
-        <v>44720.427384259259</v>
+      <c r="H12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I12" s="2"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="3">
+        <v>0</v>
+      </c>
+      <c r="M12" s="3">
+        <v>116</v>
       </c>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
@@ -1058,28 +1058,34 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
       <c r="I13" s="6"/>
-      <c r="J13" s="5"/>
+      <c r="J13" s="5" t="s">
+        <v>40</v>
+      </c>
       <c r="K13" s="6"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
+      <c r="L13" s="10">
+        <v>44582.531331018516</v>
+      </c>
+      <c r="M13" s="10">
+        <v>44720.427384259259</v>
+      </c>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
@@ -1096,10 +1102,10 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>13</v>
@@ -1110,14 +1116,14 @@
       <c r="E14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
@@ -1134,10 +1140,10 @@
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>13</v>
@@ -1172,10 +1178,10 @@
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>13</v>
@@ -1210,10 +1216,10 @@
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>13</v>
@@ -1247,11 +1253,21 @@
       <c r="Z17" s="1"/>
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="4"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="1"/>
+      <c r="A18" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
@@ -1274,20 +1290,20 @@
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
     </row>
-    <row r="19" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="2"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="10"/>
-      <c r="M19" s="10"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
@@ -1302,7 +1318,7 @@
       <c r="Y19" s="1"/>
       <c r="Z19" s="1"/>
     </row>
-    <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1314,8 +1330,8 @@
       <c r="I20" s="6"/>
       <c r="J20" s="5"/>
       <c r="K20" s="6"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
@@ -1336,14 +1352,14 @@
       <c r="C21" s="1"/>
       <c r="D21" s="2"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
@@ -1415,6 +1431,19 @@
       <c r="Z23" s="1"/>
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="4"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
@@ -1430,14 +1459,6 @@
       <c r="Z24" s="1"/>
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="2"/>
-      <c r="L25" s="3"/>
-      <c r="M25" s="3"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
@@ -1453,19 +1474,27 @@
       <c r="Z25" s="1"/>
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="N26" s="4"/>
-      <c r="O26" s="4"/>
-      <c r="P26" s="4"/>
-      <c r="Q26" s="4"/>
-      <c r="R26" s="4"/>
-      <c r="S26" s="4"/>
-      <c r="T26" s="4"/>
-      <c r="U26" s="4"/>
-      <c r="V26" s="4"/>
-      <c r="W26" s="4"/>
-      <c r="X26" s="4"/>
-      <c r="Y26" s="4"/>
-      <c r="Z26" s="4"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1"/>
+      <c r="R26" s="1"/>
+      <c r="S26" s="1"/>
+      <c r="T26" s="1"/>
+      <c r="U26" s="1"/>
+      <c r="V26" s="1"/>
+      <c r="W26" s="1"/>
+      <c r="X26" s="1"/>
+      <c r="Y26" s="1"/>
+      <c r="Z26" s="1"/>
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="N27" s="4"/>
@@ -1483,19 +1512,19 @@
       <c r="Z27" s="4"/>
     </row>
     <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="N28" s="1"/>
-      <c r="O28" s="1"/>
-      <c r="P28" s="1"/>
-      <c r="Q28" s="1"/>
-      <c r="R28" s="1"/>
-      <c r="S28" s="1"/>
-      <c r="T28" s="1"/>
-      <c r="U28" s="1"/>
-      <c r="V28" s="1"/>
-      <c r="W28" s="1"/>
-      <c r="X28" s="1"/>
-      <c r="Y28" s="1"/>
-      <c r="Z28" s="1"/>
+      <c r="N28" s="4"/>
+      <c r="O28" s="4"/>
+      <c r="P28" s="4"/>
+      <c r="Q28" s="4"/>
+      <c r="R28" s="4"/>
+      <c r="S28" s="4"/>
+      <c r="T28" s="4"/>
+      <c r="U28" s="4"/>
+      <c r="V28" s="4"/>
+      <c r="W28" s="4"/>
+      <c r="X28" s="4"/>
+      <c r="Y28" s="4"/>
+      <c r="Z28" s="4"/>
     </row>
     <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="N29" s="1"/>
@@ -1513,19 +1542,6 @@
       <c r="Z29" s="1"/>
     </row>
     <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="4"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="3"/>
-      <c r="K30" s="2"/>
-      <c r="L30" s="3"/>
-      <c r="M30" s="3"/>
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
@@ -1625,7 +1641,7 @@
       <c r="Z33" s="1"/>
     </row>
     <row r="34" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="11"/>
+      <c r="A34" s="4"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="2"/>
@@ -1653,7 +1669,7 @@
       <c r="Z34" s="1"/>
     </row>
     <row r="35" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="12"/>
+      <c r="A35" s="11"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="2"/>
@@ -1681,7 +1697,7 @@
       <c r="Z35" s="1"/>
     </row>
     <row r="36" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="11"/>
+      <c r="A36" s="12"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="2"/>
@@ -1709,7 +1725,7 @@
       <c r="Z36" s="1"/>
     </row>
     <row r="37" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="12"/>
+      <c r="A37" s="11"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="2"/>
@@ -1737,7 +1753,7 @@
       <c r="Z37" s="1"/>
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="4"/>
+      <c r="A38" s="12"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="2"/>
@@ -2689,7 +2705,7 @@
       <c r="Z71" s="1"/>
     </row>
     <row r="72" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="1"/>
+      <c r="A72" s="4"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
       <c r="D72" s="2"/>
@@ -28616,22 +28632,50 @@
       <c r="Y997" s="1"/>
       <c r="Z997" s="1"/>
     </row>
+    <row r="998" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A998" s="1"/>
+      <c r="B998" s="1"/>
+      <c r="C998" s="1"/>
+      <c r="D998" s="2"/>
+      <c r="E998" s="1"/>
+      <c r="F998" s="3"/>
+      <c r="G998" s="3"/>
+      <c r="H998" s="3"/>
+      <c r="I998" s="2"/>
+      <c r="J998" s="3"/>
+      <c r="K998" s="2"/>
+      <c r="L998" s="3"/>
+      <c r="M998" s="3"/>
+      <c r="N998" s="1"/>
+      <c r="O998" s="1"/>
+      <c r="P998" s="1"/>
+      <c r="Q998" s="1"/>
+      <c r="R998" s="1"/>
+      <c r="S998" s="1"/>
+      <c r="T998" s="1"/>
+      <c r="U998" s="1"/>
+      <c r="V998" s="1"/>
+      <c r="W998" s="1"/>
+      <c r="X998" s="1"/>
+      <c r="Y998" s="1"/>
+      <c r="Z998" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="A37:A38"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C54:C997 C30:C42 C1:C23" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C55:C998 C31:C43 C1:C24" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E30:E997 E1:E23" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E31:E998 E1:E24" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F25 F30:F997 F1:F23" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F26 F31:F998 F1:F24" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"ratio,interval"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H25 H30:H997 H1:H23" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H26 H31:H998 H1:H24" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"natural,whole,integer,real"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
standardizes metadata and removes extra column
</commit_message>
<xml_diff>
--- a/data-raw/metadata/delta_entry_catch_metadata.xlsx
+++ b/data-raw/metadata/delta_entry_catch_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-delta-entry-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{397C9274-CAED-FA4F-90F4-8D4806710293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{807F25E8-39F5-DE43-AE55-DBB7C557A72C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32580" yWindow="1620" windowWidth="17740" windowHeight="17140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -187,9 +187,6 @@
     <t>actualCount</t>
   </si>
   <si>
-    <t>Foreign key to the CAMP ProjectDescription table. For the Delta Entry RST Project, this equals 10.</t>
-  </si>
-  <si>
     <t>Delta Entry RST</t>
   </si>
   <si>
@@ -206,15 +203,6 @@
 "American shad", "Prickly sculpin")</t>
   </si>
   <si>
-    <t>Origin/production type of the fish. Levels = c("Natural", "Hatchery").</t>
-  </si>
-  <si>
-    <t>Life stage of the fish. Levels = c("Not recorded", "Button-up fry", "Parr", "Smolt", "Ammocoete", "Silvery parr", "Yolk sac fry (alevin)", "Juvenile").</t>
-  </si>
-  <si>
-    <t>Work that was done during visit to trap. Levels = c("Start trap &amp; begin trapping", "Continue trapping", "Unplanned restart", "End trapping").</t>
-  </si>
-  <si>
     <t>Name of the sampling site. Levels = "Lower Sacramento River RST"</t>
   </si>
   <si>
@@ -227,7 +215,21 @@
     <t>atCaptureRun</t>
   </si>
   <si>
-    <t>Run designation as determined in the field or as assigned at a later date. Levels = c("Not recorded", "Fall", "Spring", "Winter", "Late fall", "Not applicable (n/a)").</t>
+    <t xml:space="preserve">Foreign key to the CAMP ProjectDescription table. All data associated with this package will have a ProjectDescriptionID = 10. </t>
+  </si>
+  <si>
+    <t>Run designation as determined in the field or as assigned at a later date. Levels =c("Not recorded", "Fall", "Spring", "Winter", NA)</t>
+  </si>
+  <si>
+    <t>Origin/production type of the fish. Levels =c("Natural", "Hatchery")</t>
+  </si>
+  <si>
+    <t>Life stage of the fish. Levels = c("Not recorded", "Button-up fry", "Parr", "Smolt", "Ammocoete", 
+"Silvery parr", "Yolk sac fry (alevin)", "Juvenile")</t>
+  </si>
+  <si>
+    <t>Work that was done during visit to trap. Levels =c("Start trap &amp; begin trapping", "Continue trapping", "Unplanned restart", 
+"End trapping")</t>
   </si>
 </sst>
 </file>
@@ -534,7 +536,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -613,7 +615,7 @@
         <v>44</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>18</v>
@@ -727,7 +729,7 @@
         <v>45</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>13</v>
@@ -800,10 +802,10 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>13</v>
@@ -841,7 +843,7 @@
         <v>24</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>13</v>
@@ -879,7 +881,7 @@
         <v>25</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>13</v>
@@ -1105,7 +1107,7 @@
         <v>41</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>13</v>
@@ -1143,7 +1145,7 @@
         <v>42</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>13</v>
@@ -1181,7 +1183,7 @@
         <v>43</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>13</v>
@@ -1219,7 +1221,7 @@
         <v>51</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>13</v>
@@ -28739,7 +28741,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>44</v>

</xml_diff>